<commit_message>
ahle_sr.csv now includes current scenario output
</commit_message>
<xml_diff>
--- a/Ethiopia Workspace/Code and Control Files/Disease specific attribution/input/impact_inputs.xlsx
+++ b/Ethiopia Workspace/Code and Control Files/Disease specific attribution/input/impact_inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alarkins/Desktop/Disease specific attribution/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alarkins/Documents/GitHub/GBADsLiverpool/Ethiopia Workspace/Code and Control Files/Disease specific attribution/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8147739A-71C7-E941-95D4-00B429AE36BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3542C62-F659-E340-9A15-80784CB4950C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32300" yWindow="-60" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{BDF1304B-A11E-9F40-8E8C-E06F04432198}"/>
+    <workbookView xWindow="30240" yWindow="-620" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{BDF1304B-A11E-9F40-8E8C-E06F04432198}"/>
   </bookViews>
   <sheets>
     <sheet name="ImpactValue" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="72">
   <si>
     <t>AlphaN</t>
   </si>
@@ -200,10 +200,61 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>SR only</t>
-  </si>
-  <si>
-    <t>Cattle only</t>
+    <t>CLM_C_FMD</t>
+  </si>
+  <si>
+    <t>Past_C_FMD</t>
+  </si>
+  <si>
+    <t>PUD_C_FMD</t>
+  </si>
+  <si>
+    <t>ALL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decrease in production </t>
+  </si>
+  <si>
+    <t>ImpactValue tab are parameters where there is a known affected value. ImpactChange tab are parameters as a proportion of current production.</t>
+  </si>
+  <si>
+    <t>runif(10000,0.75,0.99)</t>
+  </si>
+  <si>
+    <t>FMD</t>
+  </si>
+  <si>
+    <t>runif(10000,0.20,0.67)*prop_lactation_affected</t>
+  </si>
+  <si>
+    <t>prop_lactation_affected</t>
+  </si>
+  <si>
+    <t>prop_lactation_affected is based on length of disease in days / length of lactation</t>
+  </si>
+  <si>
+    <t>Need to investigate if new parameters drawn each month or is one parameter applied to all months?</t>
+  </si>
+  <si>
+    <t>Is milk calculated for entire lactation at once? If so need apply length of decreased lactation for diseases</t>
+  </si>
+  <si>
+    <t>Cattle only. Birr/head/month</t>
+  </si>
+  <si>
+    <t>SR only. Birr/head/month</t>
+  </si>
+  <si>
+    <t>Is treatment expenditure applied to all treated?</t>
+  </si>
+  <si>
+    <t>runif(10000, 58/12, 165)</t>
+  </si>
+  <si>
+    <t>Prop_treated</t>
+  </si>
+  <si>
+    <t>rbeta(10000,37.2022470719595,13.3120658038028)</t>
   </si>
 </sst>
 </file>
@@ -254,11 +305,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -573,22 +625,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B16E0645-2894-FB4D-A4BB-56EC451C1758}">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="D7:F16"/>
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.1640625" customWidth="1"/>
     <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="20.5" bestFit="1" customWidth="1"/>
     <col min="7" max="13" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="21.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -628,8 +682,17 @@
       <c r="M1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N1" t="s">
+        <v>53</v>
+      </c>
+      <c r="O1" t="s">
+        <v>54</v>
+      </c>
+      <c r="P1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -666,8 +729,17 @@
       <c r="M2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N2">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="O2">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="P2">
+        <v>9.7000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -683,8 +755,17 @@
       <c r="F3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N3">
+        <v>1.9E-2</v>
+      </c>
+      <c r="O3">
+        <v>1E-3</v>
+      </c>
+      <c r="P3">
+        <v>1.9E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -721,8 +802,17 @@
       <c r="M4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N4">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="O4">
+        <v>2E-3</v>
+      </c>
+      <c r="P4">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -738,13 +828,22 @@
       <c r="F5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N5">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="O5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="P5">
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="C6" t="s">
         <v>19</v>
@@ -771,29 +870,43 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>50</v>
       </c>
-      <c r="B8" t="s">
-        <v>54</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="B9" t="s">
+        <v>66</v>
+      </c>
+      <c r="G9" t="s">
         <v>19</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H9" t="s">
         <v>19</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I9" t="s">
         <v>19</v>
+      </c>
+      <c r="N9" t="s">
+        <v>69</v>
+      </c>
+      <c r="O9" t="s">
+        <v>69</v>
+      </c>
+      <c r="P9" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -803,21 +916,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7182861-DAF9-3B49-AB75-1F81C29F88BD}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D79"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
     <col min="2" max="7" width="19.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.5" customWidth="1"/>
     <col min="9" max="12" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="44.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -854,8 +968,17 @@
       <c r="L1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" t="s">
+        <v>53</v>
+      </c>
+      <c r="N1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -893,42 +1016,82 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" t="s">
+        <v>71</v>
+      </c>
+      <c r="N3" t="s">
+        <v>71</v>
+      </c>
+      <c r="O3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="D3" t="s">
+      <c r="B4" s="1"/>
+      <c r="D4" t="s">
         <v>34</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K4" t="s">
         <v>35</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="M4" t="s">
+        <v>61</v>
+      </c>
+      <c r="N4" t="s">
+        <v>61</v>
+      </c>
+      <c r="O4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="M5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="K7" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -937,10 +1100,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4508A998-6E75-A543-8ED2-291BE3DA8BEA}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -948,7 +1111,7 @@
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="69.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -990,7 +1153,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
-        <f t="shared" ref="A3:A8" si="0">ROW()-1</f>
+        <f t="shared" ref="A3:A10" si="0">ROW()-1</f>
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -1094,6 +1257,42 @@
       </c>
       <c r="E8" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1103,17 +1302,37 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCB713E6-1F06-EE43-A353-1A5BE609FA28}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>